<commit_message>
[24.01.12 11:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI RESOURCE.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI RESOURCE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1188" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E1CD0F2-E84D-4839-9F12-1562F3524767}"/>
+  <xr:revisionPtr revIDLastSave="1197" documentId="8_{4FA08952-AD8A-4EC5-BA39-9F1D18567017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{041DE4A5-FAD7-4ACF-A48F-261D3586C397}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E3A59C1D-DF4F-40E3-A908-700669E2F1F4}"/>
   </bookViews>
   <sheets>
     <sheet name="RESOURCE.UM" sheetId="6" r:id="rId1"/>
@@ -37,6 +37,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A1A63B83-8E84-4021-B9EA-CDD31A45BF58}</author>
+  </authors>
+  <commentList>
+    <comment ref="A520" authorId="0" shapeId="0" xr:uid="{A1A63B83-8E84-4021-B9EA-CDD31A45BF58}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    VSAV</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="1968">
   <si>
@@ -5948,7 +5966,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5991,6 +6009,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -6672,6 +6696,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Daphné LECCIA (EXT)" id="{E8E91ABB-5E93-4BB0-80A4-051EFB9FFE55}" userId="S::Daphne.LECCIA.EXT@esante.gouv.fr::9cca622e-4bc3-4039-b46f-9ab4e737295d" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42A3190F-B4C4-4FD6-A2E5-527D528AB8D4}" name="Table1345791132" displayName="Table1345791132" ref="A9:E59" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A9:E59" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}"/>
@@ -6688,13 +6718,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F75B1DA5-9891-4F6A-AB67-59BFCEA39278}" name="Table134579113" displayName="Table134579113" ref="A9:F610" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A9:F610" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Véhicule"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:F610" xr:uid="{055641F3-D0AB-4717-B922-6E3A5263A366}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D3C2EF9F-0A39-4713-AB81-BA1DFEE125BD}" name="Code" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{BDEDD48A-6D09-407F-B330-F11B697A342A}" name="Libellé niveau 1" dataDxfId="10"/>
@@ -7015,6 +7039,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A520" dT="2024-01-12T09:38:27.85" personId="{E8E91ABB-5E93-4BB0-80A4-051EFB9FFE55}" id="{A1A63B83-8E84-4021-B9EA-CDD31A45BF58}">
+    <text>VSAV</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CEF5FD-1940-42EA-85AA-122B06213404}">
   <dimension ref="A1:E59"/>
@@ -7866,17 +7898,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB9E0D-B8DC-4CCE-8710-BDDD2261629F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB9E0D-B8DC-4CCE-8710-BDDD2261629F}">
   <dimension ref="A1:F610"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A312" sqref="A312"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="4" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="90.85546875" customWidth="1"/>
     <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
@@ -7977,7 +8011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>157</v>
       </c>
@@ -7991,7 +8025,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>160</v>
       </c>
@@ -8005,7 +8039,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>163</v>
       </c>
@@ -8019,7 +8053,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>166</v>
       </c>
@@ -8033,7 +8067,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>169</v>
       </c>
@@ -8049,7 +8083,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>172</v>
       </c>
@@ -8065,7 +8099,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>175</v>
       </c>
@@ -8081,7 +8115,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>178</v>
       </c>
@@ -8097,7 +8131,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>181</v>
       </c>
@@ -8113,7 +8147,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>184</v>
       </c>
@@ -8129,7 +8163,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>187</v>
       </c>
@@ -8145,7 +8179,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>190</v>
       </c>
@@ -8163,7 +8197,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>193</v>
       </c>
@@ -8181,7 +8215,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>196</v>
       </c>
@@ -8199,7 +8233,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>199</v>
       </c>
@@ -8217,7 +8251,7 @@
       </c>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>202</v>
       </c>
@@ -8235,7 +8269,7 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>205</v>
       </c>
@@ -8253,7 +8287,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>208</v>
       </c>
@@ -8271,7 +8305,7 @@
       </c>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>211</v>
       </c>
@@ -8289,7 +8323,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>214</v>
       </c>
@@ -8307,7 +8341,7 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>217</v>
       </c>
@@ -8325,7 +8359,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>220</v>
       </c>
@@ -8343,7 +8377,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>223</v>
       </c>
@@ -8361,7 +8395,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>226</v>
       </c>
@@ -8379,7 +8413,7 @@
       </c>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>229</v>
       </c>
@@ -8397,7 +8431,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>231</v>
       </c>
@@ -8415,7 +8449,7 @@
       </c>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>234</v>
       </c>
@@ -8433,7 +8467,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>237</v>
       </c>
@@ -8451,7 +8485,7 @@
       </c>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>240</v>
       </c>
@@ -8469,7 +8503,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>243</v>
       </c>
@@ -8487,7 +8521,7 @@
       </c>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>246</v>
       </c>
@@ -8505,7 +8539,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>249</v>
       </c>
@@ -8523,7 +8557,7 @@
       </c>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>252</v>
       </c>
@@ -8541,7 +8575,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>255</v>
       </c>
@@ -8559,7 +8593,7 @@
       </c>
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>258</v>
       </c>
@@ -8577,7 +8611,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>261</v>
       </c>
@@ -8595,7 +8629,7 @@
       </c>
       <c r="F45" s="7"/>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>264</v>
       </c>
@@ -8613,7 +8647,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>267</v>
       </c>
@@ -8631,7 +8665,7 @@
       </c>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>270</v>
       </c>
@@ -8649,7 +8683,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>273</v>
       </c>
@@ -8667,7 +8701,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>276</v>
       </c>
@@ -8685,7 +8719,7 @@
       </c>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>279</v>
       </c>
@@ -8703,7 +8737,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>282</v>
       </c>
@@ -8721,7 +8755,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>285</v>
       </c>
@@ -8739,7 +8773,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>288</v>
       </c>
@@ -8757,7 +8791,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>291</v>
       </c>
@@ -8775,7 +8809,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>294</v>
       </c>
@@ -8793,7 +8827,7 @@
       </c>
       <c r="F56" s="7"/>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>296</v>
       </c>
@@ -8811,7 +8845,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>299</v>
       </c>
@@ -8829,7 +8863,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>301</v>
       </c>
@@ -8847,7 +8881,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>304</v>
       </c>
@@ -8865,7 +8899,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>307</v>
       </c>
@@ -8883,7 +8917,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>310</v>
       </c>
@@ -8901,7 +8935,7 @@
       </c>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>313</v>
       </c>
@@ -8919,7 +8953,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>316</v>
       </c>
@@ -8937,7 +8971,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>319</v>
       </c>
@@ -8955,7 +8989,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>322</v>
       </c>
@@ -8973,7 +9007,7 @@
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>325</v>
       </c>
@@ -8991,7 +9025,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>328</v>
       </c>
@@ -9009,7 +9043,7 @@
       </c>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>330</v>
       </c>
@@ -9027,7 +9061,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>333</v>
       </c>
@@ -9045,7 +9079,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>335</v>
       </c>
@@ -9063,7 +9097,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>338</v>
       </c>
@@ -9081,7 +9115,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>341</v>
       </c>
@@ -9099,7 +9133,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>344</v>
       </c>
@@ -9117,7 +9151,7 @@
       </c>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>347</v>
       </c>
@@ -9135,7 +9169,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>350</v>
       </c>
@@ -9153,7 +9187,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>353</v>
       </c>
@@ -9171,7 +9205,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>356</v>
       </c>
@@ -9189,7 +9223,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>358</v>
       </c>
@@ -9207,7 +9241,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>361</v>
       </c>
@@ -9225,7 +9259,7 @@
       </c>
       <c r="F80" s="7"/>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>363</v>
       </c>
@@ -9243,7 +9277,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>366</v>
       </c>
@@ -9261,7 +9295,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>369</v>
       </c>
@@ -9279,7 +9313,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>372</v>
       </c>
@@ -9297,7 +9331,7 @@
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>375</v>
       </c>
@@ -9315,7 +9349,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>378</v>
       </c>
@@ -9333,7 +9367,7 @@
       </c>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>381</v>
       </c>
@@ -9351,7 +9385,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>384</v>
       </c>
@@ -9369,7 +9403,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>386</v>
       </c>
@@ -9387,7 +9421,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>389</v>
       </c>
@@ -9405,7 +9439,7 @@
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>392</v>
       </c>
@@ -9423,7 +9457,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>395</v>
       </c>
@@ -9441,7 +9475,7 @@
       </c>
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>398</v>
       </c>
@@ -9459,7 +9493,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>401</v>
       </c>
@@ -9477,7 +9511,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>404</v>
       </c>
@@ -9495,7 +9529,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>407</v>
       </c>
@@ -9513,7 +9547,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>410</v>
       </c>
@@ -9531,7 +9565,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>413</v>
       </c>
@@ -9549,7 +9583,7 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>416</v>
       </c>
@@ -9567,7 +9601,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>419</v>
       </c>
@@ -9585,7 +9619,7 @@
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>422</v>
       </c>
@@ -9603,7 +9637,7 @@
       </c>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>425</v>
       </c>
@@ -9621,7 +9655,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>428</v>
       </c>
@@ -9639,7 +9673,7 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>431</v>
       </c>
@@ -9657,7 +9691,7 @@
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>434</v>
       </c>
@@ -9675,7 +9709,7 @@
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>437</v>
       </c>
@@ -9693,7 +9727,7 @@
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>439</v>
       </c>
@@ -9711,7 +9745,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>442</v>
       </c>
@@ -9729,7 +9763,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>442</v>
       </c>
@@ -9747,7 +9781,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>447</v>
       </c>
@@ -9765,7 +9799,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>450</v>
       </c>
@@ -9783,7 +9817,7 @@
       </c>
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>453</v>
       </c>
@@ -9801,7 +9835,7 @@
       </c>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>456</v>
       </c>
@@ -9819,7 +9853,7 @@
       </c>
       <c r="F113" s="7"/>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>459</v>
       </c>
@@ -9837,7 +9871,7 @@
       </c>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>462</v>
       </c>
@@ -9855,7 +9889,7 @@
       </c>
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>465</v>
       </c>
@@ -9873,7 +9907,7 @@
       </c>
       <c r="F116" s="7"/>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>468</v>
       </c>
@@ -9891,7 +9925,7 @@
       </c>
       <c r="F117" s="7"/>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>471</v>
       </c>
@@ -9909,7 +9943,7 @@
       </c>
       <c r="F118" s="7"/>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>474</v>
       </c>
@@ -9927,7 +9961,7 @@
       </c>
       <c r="F119" s="7"/>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>477</v>
       </c>
@@ -9945,7 +9979,7 @@
       </c>
       <c r="F120" s="7"/>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>480</v>
       </c>
@@ -9963,7 +9997,7 @@
       </c>
       <c r="F121" s="7"/>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>483</v>
       </c>
@@ -9981,7 +10015,7 @@
       </c>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>486</v>
       </c>
@@ -9999,7 +10033,7 @@
       </c>
       <c r="F123" s="7"/>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>489</v>
       </c>
@@ -10017,7 +10051,7 @@
       </c>
       <c r="F124" s="7"/>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>492</v>
       </c>
@@ -10035,7 +10069,7 @@
       </c>
       <c r="F125" s="7"/>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>495</v>
       </c>
@@ -10053,7 +10087,7 @@
       </c>
       <c r="F126" s="7"/>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>498</v>
       </c>
@@ -10071,7 +10105,7 @@
       </c>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>501</v>
       </c>
@@ -10089,7 +10123,7 @@
       </c>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>504</v>
       </c>
@@ -10107,7 +10141,7 @@
       </c>
       <c r="F129" s="7"/>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>507</v>
       </c>
@@ -10125,7 +10159,7 @@
       </c>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>510</v>
       </c>
@@ -10143,7 +10177,7 @@
       </c>
       <c r="F131" s="7"/>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>513</v>
       </c>
@@ -10161,7 +10195,7 @@
       </c>
       <c r="F132" s="7"/>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>516</v>
       </c>
@@ -10179,7 +10213,7 @@
       </c>
       <c r="F133" s="7"/>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>519</v>
       </c>
@@ -10197,7 +10231,7 @@
       </c>
       <c r="F134" s="7"/>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>522</v>
       </c>
@@ -10215,7 +10249,7 @@
       </c>
       <c r="F135" s="7"/>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>525</v>
       </c>
@@ -10233,7 +10267,7 @@
       </c>
       <c r="F136" s="7"/>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>528</v>
       </c>
@@ -10251,7 +10285,7 @@
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>531</v>
       </c>
@@ -10269,7 +10303,7 @@
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>534</v>
       </c>
@@ -10287,7 +10321,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>537</v>
       </c>
@@ -10305,7 +10339,7 @@
       </c>
       <c r="F140" s="7"/>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>540</v>
       </c>
@@ -10323,7 +10357,7 @@
       </c>
       <c r="F141" s="7"/>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>543</v>
       </c>
@@ -10341,7 +10375,7 @@
       </c>
       <c r="F142" s="7"/>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>546</v>
       </c>
@@ -10359,7 +10393,7 @@
       </c>
       <c r="F143" s="7"/>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>549</v>
       </c>
@@ -10377,7 +10411,7 @@
       </c>
       <c r="F144" s="7"/>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>552</v>
       </c>
@@ -10395,7 +10429,7 @@
       </c>
       <c r="F145" s="7"/>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>555</v>
       </c>
@@ -10413,7 +10447,7 @@
       </c>
       <c r="F146" s="7"/>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>558</v>
       </c>
@@ -10431,7 +10465,7 @@
       </c>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>561</v>
       </c>
@@ -10449,7 +10483,7 @@
       </c>
       <c r="F148" s="7"/>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>564</v>
       </c>
@@ -10467,7 +10501,7 @@
       </c>
       <c r="F149" s="7"/>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>567</v>
       </c>
@@ -10485,7 +10519,7 @@
       </c>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>570</v>
       </c>
@@ -10503,7 +10537,7 @@
       </c>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>573</v>
       </c>
@@ -10521,7 +10555,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>576</v>
       </c>
@@ -10539,7 +10573,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>579</v>
       </c>
@@ -10557,7 +10591,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>582</v>
       </c>
@@ -10575,7 +10609,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>585</v>
       </c>
@@ -10591,7 +10625,7 @@
       </c>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>588</v>
       </c>
@@ -10607,7 +10641,7 @@
       </c>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>591</v>
       </c>
@@ -10623,7 +10657,7 @@
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>594</v>
       </c>
@@ -10641,7 +10675,7 @@
       </c>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>597</v>
       </c>
@@ -10659,7 +10693,7 @@
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>600</v>
       </c>
@@ -10677,7 +10711,7 @@
       </c>
       <c r="F161" s="7"/>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>603</v>
       </c>
@@ -10695,7 +10729,7 @@
       </c>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>606</v>
       </c>
@@ -10713,7 +10747,7 @@
       </c>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>609</v>
       </c>
@@ -10731,7 +10765,7 @@
       </c>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>612</v>
       </c>
@@ -10749,7 +10783,7 @@
       </c>
       <c r="F165" s="7"/>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>615</v>
       </c>
@@ -10767,7 +10801,7 @@
       </c>
       <c r="F166" s="7"/>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>618</v>
       </c>
@@ -10785,7 +10819,7 @@
       </c>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>621</v>
       </c>
@@ -10803,7 +10837,7 @@
       </c>
       <c r="F168" s="7"/>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>624</v>
       </c>
@@ -10821,7 +10855,7 @@
       </c>
       <c r="F169" s="7"/>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>627</v>
       </c>
@@ -10839,7 +10873,7 @@
       </c>
       <c r="F170" s="7"/>
     </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>630</v>
       </c>
@@ -10857,7 +10891,7 @@
       </c>
       <c r="F171" s="7"/>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>633</v>
       </c>
@@ -10875,7 +10909,7 @@
       </c>
       <c r="F172" s="7"/>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
         <v>636</v>
       </c>
@@ -10893,7 +10927,7 @@
       </c>
       <c r="F173" s="7"/>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>639</v>
       </c>
@@ -10911,7 +10945,7 @@
       </c>
       <c r="F174" s="7"/>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
         <v>642</v>
       </c>
@@ -10929,7 +10963,7 @@
       </c>
       <c r="F175" s="7"/>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
         <v>645</v>
       </c>
@@ -10947,7 +10981,7 @@
       </c>
       <c r="F176" s="7"/>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>648</v>
       </c>
@@ -10965,7 +10999,7 @@
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>651</v>
       </c>
@@ -10983,7 +11017,7 @@
       </c>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>654</v>
       </c>
@@ -11001,7 +11035,7 @@
       </c>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>657</v>
       </c>
@@ -11019,7 +11053,7 @@
       </c>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>660</v>
       </c>
@@ -11037,7 +11071,7 @@
       </c>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>663</v>
       </c>
@@ -11055,7 +11089,7 @@
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>666</v>
       </c>
@@ -11073,7 +11107,7 @@
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>669</v>
       </c>
@@ -11091,7 +11125,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
         <v>672</v>
       </c>
@@ -11109,7 +11143,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
         <v>675</v>
       </c>
@@ -11127,7 +11161,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
         <v>678</v>
       </c>
@@ -11145,7 +11179,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>681</v>
       </c>
@@ -11163,7 +11197,7 @@
       </c>
       <c r="F188" s="7"/>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>684</v>
       </c>
@@ -11181,7 +11215,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>687</v>
       </c>
@@ -11199,7 +11233,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>690</v>
       </c>
@@ -11217,7 +11251,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>693</v>
       </c>
@@ -11235,7 +11269,7 @@
       </c>
       <c r="F192" s="7"/>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>696</v>
       </c>
@@ -11253,7 +11287,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>699</v>
       </c>
@@ -11271,7 +11305,7 @@
       </c>
       <c r="F194" s="7"/>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
         <v>702</v>
       </c>
@@ -11289,7 +11323,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>705</v>
       </c>
@@ -11307,7 +11341,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>708</v>
       </c>
@@ -11325,7 +11359,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>711</v>
       </c>
@@ -11343,7 +11377,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>714</v>
       </c>
@@ -11361,7 +11395,7 @@
       </c>
       <c r="F199" s="7"/>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>717</v>
       </c>
@@ -11379,7 +11413,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>720</v>
       </c>
@@ -11397,7 +11431,7 @@
       </c>
       <c r="F201" s="7"/>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>723</v>
       </c>
@@ -11415,7 +11449,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>726</v>
       </c>
@@ -11433,7 +11467,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>729</v>
       </c>
@@ -11451,7 +11485,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
         <v>732</v>
       </c>
@@ -11469,7 +11503,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>735</v>
       </c>
@@ -11487,7 +11521,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
         <v>737</v>
       </c>
@@ -11505,7 +11539,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>740</v>
       </c>
@@ -11523,7 +11557,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
         <v>743</v>
       </c>
@@ -11541,7 +11575,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
         <v>746</v>
       </c>
@@ -11559,7 +11593,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
         <v>749</v>
       </c>
@@ -11577,7 +11611,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>752</v>
       </c>
@@ -11595,7 +11629,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>755</v>
       </c>
@@ -11613,7 +11647,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>758</v>
       </c>
@@ -11631,7 +11665,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>761</v>
       </c>
@@ -11649,7 +11683,7 @@
       </c>
       <c r="F215" s="7"/>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
         <v>764</v>
       </c>
@@ -11667,7 +11701,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
         <v>767</v>
       </c>
@@ -11685,7 +11719,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
         <v>770</v>
       </c>
@@ -11703,7 +11737,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
         <v>773</v>
       </c>
@@ -11721,7 +11755,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
         <v>776</v>
       </c>
@@ -11739,7 +11773,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
         <v>779</v>
       </c>
@@ -11757,7 +11791,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
         <v>782</v>
       </c>
@@ -11775,7 +11809,7 @@
       </c>
       <c r="F222" s="7"/>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
         <v>785</v>
       </c>
@@ -11793,7 +11827,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
         <v>788</v>
       </c>
@@ -11811,7 +11845,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
         <v>791</v>
       </c>
@@ -11829,7 +11863,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>794</v>
       </c>
@@ -11847,7 +11881,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
         <v>797</v>
       </c>
@@ -11865,7 +11899,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
         <v>800</v>
       </c>
@@ -11883,7 +11917,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
         <v>803</v>
       </c>
@@ -11901,7 +11935,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
         <v>806</v>
       </c>
@@ -11919,7 +11953,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
         <v>809</v>
       </c>
@@ -11937,7 +11971,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
         <v>812</v>
       </c>
@@ -11955,7 +11989,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
         <v>815</v>
       </c>
@@ -11973,7 +12007,7 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
         <v>818</v>
       </c>
@@ -11991,7 +12025,7 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
         <v>821</v>
       </c>
@@ -12009,7 +12043,7 @@
       </c>
       <c r="F235" s="7"/>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
         <v>824</v>
       </c>
@@ -12027,7 +12061,7 @@
       </c>
       <c r="F236" s="7"/>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
         <v>827</v>
       </c>
@@ -12045,7 +12079,7 @@
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
         <v>830</v>
       </c>
@@ -12063,7 +12097,7 @@
       </c>
       <c r="F238" s="7"/>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
         <v>833</v>
       </c>
@@ -12081,7 +12115,7 @@
       </c>
       <c r="F239" s="7"/>
     </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
         <v>836</v>
       </c>
@@ -12099,7 +12133,7 @@
       </c>
       <c r="F240" s="7"/>
     </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
         <v>839</v>
       </c>
@@ -12117,7 +12151,7 @@
       </c>
       <c r="F241" s="7"/>
     </row>
-    <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
         <v>842</v>
       </c>
@@ -12135,7 +12169,7 @@
       </c>
       <c r="F242" s="7"/>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
         <v>845</v>
       </c>
@@ -12153,7 +12187,7 @@
       </c>
       <c r="F243" s="7"/>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
         <v>848</v>
       </c>
@@ -12171,7 +12205,7 @@
       </c>
       <c r="F244" s="7"/>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
         <v>851</v>
       </c>
@@ -12189,7 +12223,7 @@
       </c>
       <c r="F245" s="7"/>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
         <v>854</v>
       </c>
@@ -12207,7 +12241,7 @@
       </c>
       <c r="F246" s="7"/>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
         <v>857</v>
       </c>
@@ -12225,7 +12259,7 @@
       </c>
       <c r="F247" s="7"/>
     </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="7" t="s">
         <v>860</v>
       </c>
@@ -12243,7 +12277,7 @@
       </c>
       <c r="F248" s="7"/>
     </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
         <v>863</v>
       </c>
@@ -12261,7 +12295,7 @@
       </c>
       <c r="F249" s="7"/>
     </row>
-    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="7" t="s">
         <v>866</v>
       </c>
@@ -12279,7 +12313,7 @@
       </c>
       <c r="F250" s="7"/>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="7" t="s">
         <v>869</v>
       </c>
@@ -12297,7 +12331,7 @@
       </c>
       <c r="F251" s="7"/>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="7" t="s">
         <v>872</v>
       </c>
@@ -12315,7 +12349,7 @@
       </c>
       <c r="F252" s="7"/>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="7" t="s">
         <v>875</v>
       </c>
@@ -12333,7 +12367,7 @@
       </c>
       <c r="F253" s="7"/>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="7" t="s">
         <v>878</v>
       </c>
@@ -12351,7 +12385,7 @@
       </c>
       <c r="F254" s="7"/>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="7" t="s">
         <v>881</v>
       </c>
@@ -12369,7 +12403,7 @@
       </c>
       <c r="F255" s="7"/>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="7" t="s">
         <v>884</v>
       </c>
@@ -12387,7 +12421,7 @@
       </c>
       <c r="F256" s="7"/>
     </row>
-    <row r="257" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="7" t="s">
         <v>887</v>
       </c>
@@ -12405,7 +12439,7 @@
       </c>
       <c r="F257" s="7"/>
     </row>
-    <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="7" t="s">
         <v>890</v>
       </c>
@@ -12423,7 +12457,7 @@
       </c>
       <c r="F258" s="7"/>
     </row>
-    <row r="259" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="7" t="s">
         <v>893</v>
       </c>
@@ -12441,7 +12475,7 @@
       </c>
       <c r="F259" s="7"/>
     </row>
-    <row r="260" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="7" t="s">
         <v>896</v>
       </c>
@@ -12459,7 +12493,7 @@
       </c>
       <c r="F260" s="7"/>
     </row>
-    <row r="261" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
         <v>899</v>
       </c>
@@ -12477,7 +12511,7 @@
       </c>
       <c r="F261" s="7"/>
     </row>
-    <row r="262" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="7" t="s">
         <v>902</v>
       </c>
@@ -12495,7 +12529,7 @@
       </c>
       <c r="F262" s="7"/>
     </row>
-    <row r="263" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
         <v>905</v>
       </c>
@@ -12513,7 +12547,7 @@
       </c>
       <c r="F263" s="7"/>
     </row>
-    <row r="264" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="7" t="s">
         <v>908</v>
       </c>
@@ -12531,7 +12565,7 @@
       </c>
       <c r="F264" s="7"/>
     </row>
-    <row r="265" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="7" t="s">
         <v>911</v>
       </c>
@@ -12549,7 +12583,7 @@
       </c>
       <c r="F265" s="7"/>
     </row>
-    <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="7" t="s">
         <v>914</v>
       </c>
@@ -12567,7 +12601,7 @@
       </c>
       <c r="F266" s="7"/>
     </row>
-    <row r="267" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="7" t="s">
         <v>917</v>
       </c>
@@ -12585,7 +12619,7 @@
       </c>
       <c r="F267" s="7"/>
     </row>
-    <row r="268" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="7" t="s">
         <v>920</v>
       </c>
@@ -12603,7 +12637,7 @@
       </c>
       <c r="F268" s="7"/>
     </row>
-    <row r="269" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="7" t="s">
         <v>923</v>
       </c>
@@ -12621,7 +12655,7 @@
       </c>
       <c r="F269" s="7"/>
     </row>
-    <row r="270" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="7" t="s">
         <v>926</v>
       </c>
@@ -12639,7 +12673,7 @@
       </c>
       <c r="F270" s="7"/>
     </row>
-    <row r="271" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="7" t="s">
         <v>929</v>
       </c>
@@ -12657,7 +12691,7 @@
       </c>
       <c r="F271" s="7"/>
     </row>
-    <row r="272" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="7" t="s">
         <v>932</v>
       </c>
@@ -12675,7 +12709,7 @@
       </c>
       <c r="F272" s="7"/>
     </row>
-    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
         <v>935</v>
       </c>
@@ -12693,7 +12727,7 @@
       </c>
       <c r="F273" s="7"/>
     </row>
-    <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="7" t="s">
         <v>938</v>
       </c>
@@ -12711,7 +12745,7 @@
       </c>
       <c r="F274" s="7"/>
     </row>
-    <row r="275" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="7" t="s">
         <v>941</v>
       </c>
@@ -12729,7 +12763,7 @@
       </c>
       <c r="F275" s="7"/>
     </row>
-    <row r="276" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="7" t="s">
         <v>944</v>
       </c>
@@ -12747,7 +12781,7 @@
       </c>
       <c r="F276" s="7"/>
     </row>
-    <row r="277" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="7" t="s">
         <v>947</v>
       </c>
@@ -12765,7 +12799,7 @@
       </c>
       <c r="F277" s="7"/>
     </row>
-    <row r="278" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="7" t="s">
         <v>950</v>
       </c>
@@ -12783,7 +12817,7 @@
       </c>
       <c r="F278" s="7"/>
     </row>
-    <row r="279" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="7" t="s">
         <v>953</v>
       </c>
@@ -12801,7 +12835,7 @@
       </c>
       <c r="F279" s="7"/>
     </row>
-    <row r="280" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="7" t="s">
         <v>954</v>
       </c>
@@ -12819,7 +12853,7 @@
       </c>
       <c r="F280" s="7"/>
     </row>
-    <row r="281" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="7" t="s">
         <v>957</v>
       </c>
@@ -12837,7 +12871,7 @@
       </c>
       <c r="F281" s="7"/>
     </row>
-    <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="7" t="s">
         <v>960</v>
       </c>
@@ -12855,7 +12889,7 @@
       </c>
       <c r="F282" s="7"/>
     </row>
-    <row r="283" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="7" t="s">
         <v>963</v>
       </c>
@@ -12873,7 +12907,7 @@
       </c>
       <c r="F283" s="7"/>
     </row>
-    <row r="284" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="7" t="s">
         <v>966</v>
       </c>
@@ -12891,7 +12925,7 @@
       </c>
       <c r="F284" s="7"/>
     </row>
-    <row r="285" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="7" t="s">
         <v>969</v>
       </c>
@@ -12909,7 +12943,7 @@
       </c>
       <c r="F285" s="7"/>
     </row>
-    <row r="286" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="7" t="s">
         <v>972</v>
       </c>
@@ -12927,7 +12961,7 @@
       </c>
       <c r="F286" s="7"/>
     </row>
-    <row r="287" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="7" t="s">
         <v>975</v>
       </c>
@@ -12945,7 +12979,7 @@
       </c>
       <c r="F287" s="7"/>
     </row>
-    <row r="288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="7" t="s">
         <v>978</v>
       </c>
@@ -12963,7 +12997,7 @@
       </c>
       <c r="F288" s="7"/>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="7" t="s">
         <v>981</v>
       </c>
@@ -12981,7 +13015,7 @@
       </c>
       <c r="F289" s="7"/>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="7" t="s">
         <v>984</v>
       </c>
@@ -12999,7 +13033,7 @@
       </c>
       <c r="F290" s="7"/>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="7" t="s">
         <v>987</v>
       </c>
@@ -13017,7 +13051,7 @@
       </c>
       <c r="F291" s="7"/>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="7" t="s">
         <v>990</v>
       </c>
@@ -13035,7 +13069,7 @@
       </c>
       <c r="F292" s="7"/>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="7" t="s">
         <v>993</v>
       </c>
@@ -13053,7 +13087,7 @@
       </c>
       <c r="F293" s="7"/>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="7" t="s">
         <v>996</v>
       </c>
@@ -13071,7 +13105,7 @@
       </c>
       <c r="F294" s="7"/>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="7" t="s">
         <v>999</v>
       </c>
@@ -13089,7 +13123,7 @@
       </c>
       <c r="F295" s="7"/>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="7" t="s">
         <v>1002</v>
       </c>
@@ -13107,7 +13141,7 @@
       </c>
       <c r="F296" s="7"/>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="7" t="s">
         <v>1005</v>
       </c>
@@ -13125,7 +13159,7 @@
       </c>
       <c r="F297" s="7"/>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="7" t="s">
         <v>1008</v>
       </c>
@@ -13143,7 +13177,7 @@
       </c>
       <c r="F298" s="7"/>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="7" t="s">
         <v>1011</v>
       </c>
@@ -13161,7 +13195,7 @@
       </c>
       <c r="F299" s="7"/>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="7" t="s">
         <v>1014</v>
       </c>
@@ -13179,7 +13213,7 @@
       </c>
       <c r="F300" s="7"/>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="7" t="s">
         <v>1017</v>
       </c>
@@ -13197,7 +13231,7 @@
       </c>
       <c r="F301" s="7"/>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="7" t="s">
         <v>1020</v>
       </c>
@@ -13215,7 +13249,7 @@
       </c>
       <c r="F302" s="7"/>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="7" t="s">
         <v>1023</v>
       </c>
@@ -13231,7 +13265,7 @@
       <c r="E303" s="7"/>
       <c r="F303" s="7"/>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="7" t="s">
         <v>1025</v>
       </c>
@@ -13249,7 +13283,7 @@
       </c>
       <c r="F304" s="7"/>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="7" t="s">
         <v>1028</v>
       </c>
@@ -13267,7 +13301,7 @@
       </c>
       <c r="F305" s="7"/>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="7" t="s">
         <v>1031</v>
       </c>
@@ -13285,7 +13319,7 @@
       </c>
       <c r="F306" s="7"/>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="7" t="s">
         <v>1034</v>
       </c>
@@ -13303,7 +13337,7 @@
       </c>
       <c r="F307" s="7"/>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="7" t="s">
         <v>1037</v>
       </c>
@@ -13321,7 +13355,7 @@
       </c>
       <c r="F308" s="7"/>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="7" t="s">
         <v>1040</v>
       </c>
@@ -13339,7 +13373,7 @@
       </c>
       <c r="F309" s="7"/>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="7" t="s">
         <v>1043</v>
       </c>
@@ -13357,7 +13391,7 @@
       </c>
       <c r="F310" s="7"/>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="7" t="s">
         <v>1046</v>
       </c>
@@ -13393,7 +13427,7 @@
       </c>
       <c r="F312" s="7"/>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="7" t="s">
         <v>1052</v>
       </c>
@@ -13411,7 +13445,7 @@
       </c>
       <c r="F313" s="7"/>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="7" t="s">
         <v>1055</v>
       </c>
@@ -13429,7 +13463,7 @@
       </c>
       <c r="F314" s="7"/>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="7" t="s">
         <v>1058</v>
       </c>
@@ -13447,7 +13481,7 @@
       </c>
       <c r="F315" s="7"/>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="7" t="s">
         <v>1061</v>
       </c>
@@ -13465,7 +13499,7 @@
       </c>
       <c r="F316" s="7"/>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="7" t="s">
         <v>1064</v>
       </c>
@@ -13483,7 +13517,7 @@
       </c>
       <c r="F317" s="7"/>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="7" t="s">
         <v>1067</v>
       </c>
@@ -13501,7 +13535,7 @@
       </c>
       <c r="F318" s="7"/>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="7" t="s">
         <v>1070</v>
       </c>
@@ -13519,7 +13553,7 @@
       </c>
       <c r="F319" s="7"/>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="7" t="s">
         <v>1073</v>
       </c>
@@ -13537,7 +13571,7 @@
       </c>
       <c r="F320" s="7"/>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="7" t="s">
         <v>1076</v>
       </c>
@@ -13555,7 +13589,7 @@
       </c>
       <c r="F321" s="7"/>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="7" t="s">
         <v>1079</v>
       </c>
@@ -13573,7 +13607,7 @@
       </c>
       <c r="F322" s="7"/>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="7" t="s">
         <v>1082</v>
       </c>
@@ -13591,7 +13625,7 @@
       </c>
       <c r="F323" s="7"/>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="7" t="s">
         <v>1085</v>
       </c>
@@ -13609,7 +13643,7 @@
       </c>
       <c r="F324" s="7"/>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="7" t="s">
         <v>1088</v>
       </c>
@@ -13627,7 +13661,7 @@
       </c>
       <c r="F325" s="7"/>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="7" t="s">
         <v>1091</v>
       </c>
@@ -13645,7 +13679,7 @@
       </c>
       <c r="F326" s="7"/>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="7" t="s">
         <v>1094</v>
       </c>
@@ -13663,7 +13697,7 @@
       </c>
       <c r="F327" s="7"/>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="7" t="s">
         <v>1097</v>
       </c>
@@ -13681,7 +13715,7 @@
       </c>
       <c r="F328" s="7"/>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="7" t="s">
         <v>1100</v>
       </c>
@@ -13699,7 +13733,7 @@
       </c>
       <c r="F329" s="7"/>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="7" t="s">
         <v>1103</v>
       </c>
@@ -13717,7 +13751,7 @@
       </c>
       <c r="F330" s="7"/>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="7" t="s">
         <v>1106</v>
       </c>
@@ -13735,7 +13769,7 @@
       </c>
       <c r="F331" s="7"/>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="7" t="s">
         <v>1109</v>
       </c>
@@ -13753,7 +13787,7 @@
       </c>
       <c r="F332" s="7"/>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="7" t="s">
         <v>1112</v>
       </c>
@@ -13771,7 +13805,7 @@
       </c>
       <c r="F333" s="7"/>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="7" t="s">
         <v>1115</v>
       </c>
@@ -13789,7 +13823,7 @@
       </c>
       <c r="F334" s="7"/>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="7" t="s">
         <v>1118</v>
       </c>
@@ -13807,7 +13841,7 @@
       </c>
       <c r="F335" s="7"/>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="7" t="s">
         <v>1121</v>
       </c>
@@ -13825,7 +13859,7 @@
       </c>
       <c r="F336" s="7"/>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" s="7" t="s">
         <v>1124</v>
       </c>
@@ -13843,7 +13877,7 @@
       </c>
       <c r="F337" s="7"/>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" s="7" t="s">
         <v>1127</v>
       </c>
@@ -13861,7 +13895,7 @@
       </c>
       <c r="F338" s="7"/>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" s="7" t="s">
         <v>1130</v>
       </c>
@@ -13879,7 +13913,7 @@
       </c>
       <c r="F339" s="7"/>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" s="7" t="s">
         <v>1133</v>
       </c>
@@ -13897,7 +13931,7 @@
       </c>
       <c r="F340" s="7"/>
     </row>
-    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" s="7" t="s">
         <v>1136</v>
       </c>
@@ -13915,7 +13949,7 @@
       </c>
       <c r="F341" s="7"/>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" s="7" t="s">
         <v>1139</v>
       </c>
@@ -13933,7 +13967,7 @@
       </c>
       <c r="F342" s="7"/>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" s="7" t="s">
         <v>1142</v>
       </c>
@@ -13951,7 +13985,7 @@
       </c>
       <c r="F343" s="7"/>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" s="7" t="s">
         <v>1145</v>
       </c>
@@ -13969,7 +14003,7 @@
       </c>
       <c r="F344" s="7"/>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" s="7" t="s">
         <v>1148</v>
       </c>
@@ -13987,7 +14021,7 @@
       </c>
       <c r="F345" s="7"/>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" s="7" t="s">
         <v>1151</v>
       </c>
@@ -14005,7 +14039,7 @@
       </c>
       <c r="F346" s="7"/>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" s="7" t="s">
         <v>1154</v>
       </c>
@@ -14023,7 +14057,7 @@
       </c>
       <c r="F347" s="7"/>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" s="7" t="s">
         <v>1157</v>
       </c>
@@ -14041,7 +14075,7 @@
       </c>
       <c r="F348" s="7"/>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" s="7" t="s">
         <v>1160</v>
       </c>
@@ -14059,7 +14093,7 @@
       </c>
       <c r="F349" s="7"/>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="7" t="s">
         <v>1162</v>
       </c>
@@ -14077,7 +14111,7 @@
       </c>
       <c r="F350" s="7"/>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="7" t="s">
         <v>1165</v>
       </c>
@@ -14095,7 +14129,7 @@
       </c>
       <c r="F351" s="7"/>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" s="7" t="s">
         <v>1167</v>
       </c>
@@ -14111,7 +14145,7 @@
       <c r="E352" s="7"/>
       <c r="F352" s="7"/>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="7" t="s">
         <v>1169</v>
       </c>
@@ -14129,7 +14163,7 @@
       </c>
       <c r="F353" s="7"/>
     </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="7" t="s">
         <v>1172</v>
       </c>
@@ -14147,7 +14181,7 @@
       </c>
       <c r="F354" s="7"/>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="7" t="s">
         <v>1175</v>
       </c>
@@ -14165,7 +14199,7 @@
       </c>
       <c r="F355" s="7"/>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" s="7" t="s">
         <v>1178</v>
       </c>
@@ -14183,7 +14217,7 @@
       </c>
       <c r="F356" s="7"/>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" s="7" t="s">
         <v>1181</v>
       </c>
@@ -14201,7 +14235,7 @@
       </c>
       <c r="F357" s="7"/>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" s="7" t="s">
         <v>1184</v>
       </c>
@@ -14219,7 +14253,7 @@
       </c>
       <c r="F358" s="7"/>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="7" t="s">
         <v>1187</v>
       </c>
@@ -14237,7 +14271,7 @@
       </c>
       <c r="F359" s="7"/>
     </row>
-    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="7" t="s">
         <v>1190</v>
       </c>
@@ -14255,7 +14289,7 @@
       </c>
       <c r="F360" s="7"/>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="7" t="s">
         <v>1193</v>
       </c>
@@ -14273,7 +14307,7 @@
       </c>
       <c r="F361" s="7"/>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" s="7" t="s">
         <v>1196</v>
       </c>
@@ -14291,7 +14325,7 @@
       </c>
       <c r="F362" s="7"/>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="7" t="s">
         <v>1199</v>
       </c>
@@ -14309,7 +14343,7 @@
       </c>
       <c r="F363" s="7"/>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="7" t="s">
         <v>1202</v>
       </c>
@@ -14327,7 +14361,7 @@
       </c>
       <c r="F364" s="7"/>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="7" t="s">
         <v>1205</v>
       </c>
@@ -14345,7 +14379,7 @@
       </c>
       <c r="F365" s="7"/>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="7" t="s">
         <v>1208</v>
       </c>
@@ -14363,7 +14397,7 @@
       </c>
       <c r="F366" s="7"/>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="7" t="s">
         <v>1211</v>
       </c>
@@ -14381,7 +14415,7 @@
       </c>
       <c r="F367" s="7"/>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="7" t="s">
         <v>1214</v>
       </c>
@@ -14399,7 +14433,7 @@
       </c>
       <c r="F368" s="7"/>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369" s="7" t="s">
         <v>1217</v>
       </c>
@@ -14417,7 +14451,7 @@
       </c>
       <c r="F369" s="7"/>
     </row>
-    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370" s="7" t="s">
         <v>1220</v>
       </c>
@@ -14435,7 +14469,7 @@
       </c>
       <c r="F370" s="7"/>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371" s="7" t="s">
         <v>1223</v>
       </c>
@@ -14451,7 +14485,7 @@
       <c r="E371" s="7"/>
       <c r="F371" s="7"/>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372" s="7" t="s">
         <v>1225</v>
       </c>
@@ -14469,7 +14503,7 @@
       </c>
       <c r="F372" s="7"/>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373" s="7" t="s">
         <v>1228</v>
       </c>
@@ -14487,7 +14521,7 @@
       </c>
       <c r="F373" s="7"/>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374" s="7" t="s">
         <v>1231</v>
       </c>
@@ -14505,7 +14539,7 @@
       </c>
       <c r="F374" s="7"/>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375" s="7" t="s">
         <v>1234</v>
       </c>
@@ -14523,7 +14557,7 @@
       </c>
       <c r="F375" s="7"/>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376" s="7" t="s">
         <v>1237</v>
       </c>
@@ -14541,7 +14575,7 @@
       </c>
       <c r="F376" s="7"/>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377" s="7" t="s">
         <v>1240</v>
       </c>
@@ -14559,7 +14593,7 @@
       </c>
       <c r="F377" s="7"/>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378" s="7" t="s">
         <v>1243</v>
       </c>
@@ -14577,7 +14611,7 @@
       </c>
       <c r="F378" s="7"/>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379" s="7" t="s">
         <v>1246</v>
       </c>
@@ -14595,7 +14629,7 @@
       </c>
       <c r="F379" s="7"/>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380" s="7" t="s">
         <v>1249</v>
       </c>
@@ -14613,7 +14647,7 @@
       </c>
       <c r="F380" s="7"/>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381" s="7" t="s">
         <v>1252</v>
       </c>
@@ -14631,7 +14665,7 @@
       </c>
       <c r="F381" s="7"/>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382" s="7" t="s">
         <v>1255</v>
       </c>
@@ -14649,7 +14683,7 @@
       </c>
       <c r="F382" s="7"/>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383" s="7" t="s">
         <v>1258</v>
       </c>
@@ -14667,7 +14701,7 @@
       </c>
       <c r="F383" s="7"/>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384" s="7" t="s">
         <v>1261</v>
       </c>
@@ -14685,7 +14719,7 @@
       </c>
       <c r="F384" s="7"/>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385" s="7" t="s">
         <v>1264</v>
       </c>
@@ -14703,7 +14737,7 @@
       </c>
       <c r="F385" s="7"/>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386" s="7" t="s">
         <v>1267</v>
       </c>
@@ -14721,7 +14755,7 @@
       </c>
       <c r="F386" s="7"/>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387" s="7" t="s">
         <v>1270</v>
       </c>
@@ -14739,7 +14773,7 @@
       </c>
       <c r="F387" s="7"/>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388" s="7" t="s">
         <v>1273</v>
       </c>
@@ -14757,7 +14791,7 @@
       </c>
       <c r="F388" s="7"/>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389" s="7" t="s">
         <v>1276</v>
       </c>
@@ -14775,7 +14809,7 @@
       </c>
       <c r="F389" s="7"/>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390" s="7" t="s">
         <v>1279</v>
       </c>
@@ -14793,7 +14827,7 @@
       </c>
       <c r="F390" s="7"/>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" s="7" t="s">
         <v>1282</v>
       </c>
@@ -14811,7 +14845,7 @@
       </c>
       <c r="F391" s="7"/>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392" s="7" t="s">
         <v>1285</v>
       </c>
@@ -14829,7 +14863,7 @@
       </c>
       <c r="F392" s="7"/>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393" s="7" t="s">
         <v>1288</v>
       </c>
@@ -14847,7 +14881,7 @@
       </c>
       <c r="F393" s="7"/>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394" s="7" t="s">
         <v>1291</v>
       </c>
@@ -14865,7 +14899,7 @@
       </c>
       <c r="F394" s="7"/>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395" s="7" t="s">
         <v>1294</v>
       </c>
@@ -14883,7 +14917,7 @@
       </c>
       <c r="F395" s="7"/>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396" s="7" t="s">
         <v>1297</v>
       </c>
@@ -14901,7 +14935,7 @@
       </c>
       <c r="F396" s="7"/>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397" s="7" t="s">
         <v>1300</v>
       </c>
@@ -14919,7 +14953,7 @@
       </c>
       <c r="F397" s="7"/>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398" s="7" t="s">
         <v>1303</v>
       </c>
@@ -14937,7 +14971,7 @@
       </c>
       <c r="F398" s="7"/>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399" s="7" t="s">
         <v>1306</v>
       </c>
@@ -14955,7 +14989,7 @@
       </c>
       <c r="F399" s="7"/>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400" s="7" t="s">
         <v>1309</v>
       </c>
@@ -14973,7 +15007,7 @@
       </c>
       <c r="F400" s="7"/>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401" s="7" t="s">
         <v>1312</v>
       </c>
@@ -14991,7 +15025,7 @@
       </c>
       <c r="F401" s="7"/>
     </row>
-    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A402" s="7" t="s">
         <v>1315</v>
       </c>
@@ -15009,7 +15043,7 @@
       </c>
       <c r="F402" s="7"/>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403" s="7" t="s">
         <v>1318</v>
       </c>
@@ -15027,7 +15061,7 @@
       </c>
       <c r="F403" s="7"/>
     </row>
-    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A404" s="7" t="s">
         <v>1321</v>
       </c>
@@ -15045,7 +15079,7 @@
       </c>
       <c r="F404" s="7"/>
     </row>
-    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A405" s="7" t="s">
         <v>1324</v>
       </c>
@@ -15063,7 +15097,7 @@
       </c>
       <c r="F405" s="7"/>
     </row>
-    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406" s="7" t="s">
         <v>1327</v>
       </c>
@@ -15081,7 +15115,7 @@
       </c>
       <c r="F406" s="7"/>
     </row>
-    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407" s="7" t="s">
         <v>1330</v>
       </c>
@@ -15099,7 +15133,7 @@
       </c>
       <c r="F407" s="7"/>
     </row>
-    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A408" s="7" t="s">
         <v>1333</v>
       </c>
@@ -15117,7 +15151,7 @@
       </c>
       <c r="F408" s="7"/>
     </row>
-    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A409" s="7" t="s">
         <v>1336</v>
       </c>
@@ -15135,7 +15169,7 @@
       </c>
       <c r="F409" s="7"/>
     </row>
-    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A410" s="7" t="s">
         <v>1339</v>
       </c>
@@ -15153,7 +15187,7 @@
       </c>
       <c r="F410" s="7"/>
     </row>
-    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411" s="7" t="s">
         <v>1342</v>
       </c>
@@ -15171,7 +15205,7 @@
       </c>
       <c r="F411" s="7"/>
     </row>
-    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412" s="7" t="s">
         <v>1345</v>
       </c>
@@ -15189,7 +15223,7 @@
       </c>
       <c r="F412" s="7"/>
     </row>
-    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A413" s="7" t="s">
         <v>1348</v>
       </c>
@@ -15207,7 +15241,7 @@
       </c>
       <c r="F413" s="7"/>
     </row>
-    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A414" s="7" t="s">
         <v>1351</v>
       </c>
@@ -15225,7 +15259,7 @@
       </c>
       <c r="F414" s="7"/>
     </row>
-    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A415" s="7" t="s">
         <v>1354</v>
       </c>
@@ -15243,7 +15277,7 @@
       </c>
       <c r="F415" s="7"/>
     </row>
-    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A416" s="7" t="s">
         <v>1357</v>
       </c>
@@ -15261,7 +15295,7 @@
       </c>
       <c r="F416" s="7"/>
     </row>
-    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A417" s="7" t="s">
         <v>1359</v>
       </c>
@@ -15279,7 +15313,7 @@
       </c>
       <c r="F417" s="7"/>
     </row>
-    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A418" s="7" t="s">
         <v>1362</v>
       </c>
@@ -15297,7 +15331,7 @@
       </c>
       <c r="F418" s="7"/>
     </row>
-    <row r="419" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A419" s="7" t="s">
         <v>1365</v>
       </c>
@@ -15315,7 +15349,7 @@
       </c>
       <c r="F419" s="7"/>
     </row>
-    <row r="420" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A420" s="7" t="s">
         <v>1368</v>
       </c>
@@ -15333,7 +15367,7 @@
       </c>
       <c r="F420" s="7"/>
     </row>
-    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421" s="7" t="s">
         <v>1371</v>
       </c>
@@ -15351,7 +15385,7 @@
       </c>
       <c r="F421" s="7"/>
     </row>
-    <row r="422" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A422" s="7" t="s">
         <v>1374</v>
       </c>
@@ -15369,7 +15403,7 @@
       </c>
       <c r="F422" s="7"/>
     </row>
-    <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A423" s="7" t="s">
         <v>1377</v>
       </c>
@@ -15387,7 +15421,7 @@
       </c>
       <c r="F423" s="7"/>
     </row>
-    <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A424" s="7" t="s">
         <v>1380</v>
       </c>
@@ -15405,7 +15439,7 @@
       </c>
       <c r="F424" s="7"/>
     </row>
-    <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A425" s="7" t="s">
         <v>1383</v>
       </c>
@@ -15423,7 +15457,7 @@
       </c>
       <c r="F425" s="7"/>
     </row>
-    <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A426" s="7" t="s">
         <v>1386</v>
       </c>
@@ -15441,7 +15475,7 @@
       </c>
       <c r="F426" s="7"/>
     </row>
-    <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A427" s="7" t="s">
         <v>1389</v>
       </c>
@@ -15459,7 +15493,7 @@
       </c>
       <c r="F427" s="7"/>
     </row>
-    <row r="428" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A428" s="7" t="s">
         <v>1392</v>
       </c>
@@ -15477,7 +15511,7 @@
       </c>
       <c r="F428" s="7"/>
     </row>
-    <row r="429" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A429" s="7" t="s">
         <v>1395</v>
       </c>
@@ -15495,7 +15529,7 @@
       </c>
       <c r="F429" s="7"/>
     </row>
-    <row r="430" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A430" s="7" t="s">
         <v>1398</v>
       </c>
@@ -15513,7 +15547,7 @@
       </c>
       <c r="F430" s="7"/>
     </row>
-    <row r="431" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431" s="7" t="s">
         <v>1401</v>
       </c>
@@ -15531,7 +15565,7 @@
       </c>
       <c r="F431" s="7"/>
     </row>
-    <row r="432" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432" s="7" t="s">
         <v>1404</v>
       </c>
@@ -15549,7 +15583,7 @@
       </c>
       <c r="F432" s="7"/>
     </row>
-    <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433" s="7" t="s">
         <v>1407</v>
       </c>
@@ -15567,7 +15601,7 @@
       </c>
       <c r="F433" s="7"/>
     </row>
-    <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434" s="7" t="s">
         <v>1410</v>
       </c>
@@ -15585,7 +15619,7 @@
       </c>
       <c r="F434" s="7"/>
     </row>
-    <row r="435" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A435" s="7" t="s">
         <v>1413</v>
       </c>
@@ -15603,7 +15637,7 @@
       </c>
       <c r="F435" s="7"/>
     </row>
-    <row r="436" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A436" s="7" t="s">
         <v>1416</v>
       </c>
@@ -15621,7 +15655,7 @@
       </c>
       <c r="F436" s="7"/>
     </row>
-    <row r="437" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A437" s="7" t="s">
         <v>1419</v>
       </c>
@@ -15639,7 +15673,7 @@
       </c>
       <c r="F437" s="7"/>
     </row>
-    <row r="438" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438" s="7" t="s">
         <v>1422</v>
       </c>
@@ -15657,7 +15691,7 @@
       </c>
       <c r="F438" s="7"/>
     </row>
-    <row r="439" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A439" s="7" t="s">
         <v>1425</v>
       </c>
@@ -15675,7 +15709,7 @@
       </c>
       <c r="F439" s="7"/>
     </row>
-    <row r="440" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A440" s="7" t="s">
         <v>1428</v>
       </c>
@@ -15693,7 +15727,7 @@
       </c>
       <c r="F440" s="7"/>
     </row>
-    <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A441" s="7" t="s">
         <v>1431</v>
       </c>
@@ -15711,7 +15745,7 @@
       </c>
       <c r="F441" s="7"/>
     </row>
-    <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A442" s="7" t="s">
         <v>1434</v>
       </c>
@@ -15729,7 +15763,7 @@
       </c>
       <c r="F442" s="7"/>
     </row>
-    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A443" s="7" t="s">
         <v>1437</v>
       </c>
@@ -15747,7 +15781,7 @@
       </c>
       <c r="F443" s="7"/>
     </row>
-    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A444" s="7" t="s">
         <v>1440</v>
       </c>
@@ -15765,7 +15799,7 @@
       </c>
       <c r="F444" s="7"/>
     </row>
-    <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A445" s="7" t="s">
         <v>1443</v>
       </c>
@@ -15783,7 +15817,7 @@
       </c>
       <c r="F445" s="7"/>
     </row>
-    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A446" s="7" t="s">
         <v>1446</v>
       </c>
@@ -15801,7 +15835,7 @@
       </c>
       <c r="F446" s="7"/>
     </row>
-    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A447" s="7" t="s">
         <v>1449</v>
       </c>
@@ -15819,7 +15853,7 @@
       </c>
       <c r="F447" s="7"/>
     </row>
-    <row r="448" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A448" s="7" t="s">
         <v>1452</v>
       </c>
@@ -15837,7 +15871,7 @@
       </c>
       <c r="F448" s="7"/>
     </row>
-    <row r="449" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A449" s="7" t="s">
         <v>1455</v>
       </c>
@@ -15855,7 +15889,7 @@
       </c>
       <c r="F449" s="7"/>
     </row>
-    <row r="450" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A450" s="7" t="s">
         <v>1458</v>
       </c>
@@ -15873,7 +15907,7 @@
       </c>
       <c r="F450" s="7"/>
     </row>
-    <row r="451" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A451" s="7" t="s">
         <v>1461</v>
       </c>
@@ -15891,7 +15925,7 @@
       </c>
       <c r="F451" s="7"/>
     </row>
-    <row r="452" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A452" s="7" t="s">
         <v>1464</v>
       </c>
@@ -15909,7 +15943,7 @@
       </c>
       <c r="F452" s="7"/>
     </row>
-    <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453" s="7" t="s">
         <v>1467</v>
       </c>
@@ -15927,7 +15961,7 @@
       </c>
       <c r="F453" s="7"/>
     </row>
-    <row r="454" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454" s="7" t="s">
         <v>1470</v>
       </c>
@@ -15945,7 +15979,7 @@
       </c>
       <c r="F454" s="7"/>
     </row>
-    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455" s="7" t="s">
         <v>1473</v>
       </c>
@@ -15963,7 +15997,7 @@
       </c>
       <c r="F455" s="7"/>
     </row>
-    <row r="456" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456" s="7" t="s">
         <v>1476</v>
       </c>
@@ -15981,7 +16015,7 @@
       </c>
       <c r="F456" s="7"/>
     </row>
-    <row r="457" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A457" s="7" t="s">
         <v>1478</v>
       </c>
@@ -15999,7 +16033,7 @@
       </c>
       <c r="F457" s="7"/>
     </row>
-    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458" s="7" t="s">
         <v>1481</v>
       </c>
@@ -16017,7 +16051,7 @@
       </c>
       <c r="F458" s="7"/>
     </row>
-    <row r="459" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A459" s="7" t="s">
         <v>1483</v>
       </c>
@@ -16035,7 +16069,7 @@
       </c>
       <c r="F459" s="7"/>
     </row>
-    <row r="460" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460" s="7" t="s">
         <v>1486</v>
       </c>
@@ -16053,7 +16087,7 @@
       </c>
       <c r="F460" s="7"/>
     </row>
-    <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A461" s="7" t="s">
         <v>1489</v>
       </c>
@@ -16071,7 +16105,7 @@
       </c>
       <c r="F461" s="7"/>
     </row>
-    <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A462" s="7" t="s">
         <v>1492</v>
       </c>
@@ -16089,7 +16123,7 @@
       </c>
       <c r="F462" s="7"/>
     </row>
-    <row r="463" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A463" s="7" t="s">
         <v>1495</v>
       </c>
@@ -16107,7 +16141,7 @@
       </c>
       <c r="F463" s="7"/>
     </row>
-    <row r="464" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A464" s="7" t="s">
         <v>1498</v>
       </c>
@@ -16125,7 +16159,7 @@
       </c>
       <c r="F464" s="7"/>
     </row>
-    <row r="465" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A465" s="7" t="s">
         <v>1501</v>
       </c>
@@ -16143,7 +16177,7 @@
       </c>
       <c r="F465" s="7"/>
     </row>
-    <row r="466" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A466" s="7" t="s">
         <v>1504</v>
       </c>
@@ -16161,7 +16195,7 @@
       </c>
       <c r="F466" s="7"/>
     </row>
-    <row r="467" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A467" s="7" t="s">
         <v>1507</v>
       </c>
@@ -18375,7 +18409,7 @@
       </c>
       <c r="F589" s="7"/>
     </row>
-    <row r="590" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A590" s="7" t="s">
         <v>1871</v>
       </c>
@@ -18391,7 +18425,7 @@
       </c>
       <c r="F590" s="7"/>
     </row>
-    <row r="591" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A591" s="7" t="s">
         <v>1874</v>
       </c>
@@ -18407,7 +18441,7 @@
       </c>
       <c r="F591" s="7"/>
     </row>
-    <row r="592" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A592" s="7" t="s">
         <v>1877</v>
       </c>
@@ -18423,7 +18457,7 @@
       </c>
       <c r="F592" s="7"/>
     </row>
-    <row r="593" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A593" s="7" t="s">
         <v>1880</v>
       </c>
@@ -18439,7 +18473,7 @@
       </c>
       <c r="F593" s="7"/>
     </row>
-    <row r="594" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A594" s="7" t="s">
         <v>1883</v>
       </c>
@@ -18455,7 +18489,7 @@
       </c>
       <c r="F594" s="7"/>
     </row>
-    <row r="595" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A595" s="7" t="s">
         <v>1886</v>
       </c>
@@ -18471,7 +18505,7 @@
       </c>
       <c r="F595" s="7"/>
     </row>
-    <row r="596" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A596" s="7" t="s">
         <v>1889</v>
       </c>
@@ -18487,7 +18521,7 @@
       </c>
       <c r="F596" s="7"/>
     </row>
-    <row r="597" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A597" s="7" t="s">
         <v>1892</v>
       </c>
@@ -18503,7 +18537,7 @@
       </c>
       <c r="F597" s="7"/>
     </row>
-    <row r="598" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A598" s="7" t="s">
         <v>1895</v>
       </c>
@@ -18519,7 +18553,7 @@
       </c>
       <c r="F598" s="7"/>
     </row>
-    <row r="599" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A599" s="7" t="s">
         <v>1898</v>
       </c>
@@ -18535,7 +18569,7 @@
       </c>
       <c r="F599" s="7"/>
     </row>
-    <row r="600" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A600" s="7" t="s">
         <v>1901</v>
       </c>
@@ -18551,7 +18585,7 @@
       </c>
       <c r="F600" s="7"/>
     </row>
-    <row r="601" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A601" s="7" t="s">
         <v>1904</v>
       </c>
@@ -18567,7 +18601,7 @@
       </c>
       <c r="F601" s="7"/>
     </row>
-    <row r="602" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A602" s="7" t="s">
         <v>1906</v>
       </c>
@@ -18583,7 +18617,7 @@
       </c>
       <c r="F602" s="7"/>
     </row>
-    <row r="603" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A603" s="7" t="s">
         <v>1909</v>
       </c>
@@ -18599,7 +18633,7 @@
       </c>
       <c r="F603" s="7"/>
     </row>
-    <row r="604" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A604" s="7" t="s">
         <v>1912</v>
       </c>
@@ -18615,7 +18649,7 @@
       </c>
       <c r="F604" s="7"/>
     </row>
-    <row r="605" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A605" s="7" t="s">
         <v>1915</v>
       </c>
@@ -18631,7 +18665,7 @@
       </c>
       <c r="F605" s="7"/>
     </row>
-    <row r="606" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A606" s="7" t="s">
         <v>1918</v>
       </c>
@@ -18647,7 +18681,7 @@
       </c>
       <c r="F606" s="7"/>
     </row>
-    <row r="607" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A607" s="7" t="s">
         <v>1921</v>
       </c>
@@ -18663,7 +18697,7 @@
       </c>
       <c r="F607" s="7"/>
     </row>
-    <row r="608" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A608" s="7" t="s">
         <v>1924</v>
       </c>
@@ -18679,7 +18713,7 @@
       </c>
       <c r="F608" s="7"/>
     </row>
-    <row r="609" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A609" s="7" t="s">
         <v>1927</v>
       </c>
@@ -18695,7 +18729,7 @@
       </c>
       <c r="F609" s="7"/>
     </row>
-    <row r="610" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A610" s="7" t="s">
         <v>1930</v>
       </c>
@@ -18714,8 +18748,9 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -18724,15 +18759,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE995B6E-F8E3-4919-A9E0-E67EE815BFB7}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19486,7 +19521,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F600F5F0-E3F4-4CD1-B823-B0373889BA6B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AAF0A29-3F52-4C58-8342-2E5A45F6CD49}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>